<commit_message>
Updated Bus 11 AM
</commit_message>
<xml_diff>
--- a/assets/files/Bus_11.xlsx
+++ b/assets/files/Bus_11.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maikenp/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maikenp/ahm18.neic.nordforsk.org/assets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Xiaxi</t>
   </si>
@@ -79,12 +79,6 @@
   </si>
   <si>
     <t>Azab Mohamed</t>
-  </si>
-  <si>
-    <t>Bjørn</t>
-  </si>
-  <si>
-    <t>Lindi</t>
   </si>
   <si>
     <t>Michaela</t>
@@ -524,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -772,7 +766,7 @@
         <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C22" s="1">
         <v>0.45833333333333331</v>
@@ -783,20 +777,9 @@
         <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C23" s="1">
-        <v>0.45833333333333331</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="1">
         <v>0.45833333333333331</v>
       </c>
     </row>

</xml_diff>